<commit_message>
Updating notebook and files from 5/18
</commit_message>
<xml_diff>
--- a/analysis/analysis_innnings.xlsx
+++ b/analysis/analysis_innnings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E599"/>
+  <dimension ref="A1:E623"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13880,20 +13880,16 @@
           <t>New York Yankees</t>
         </is>
       </c>
-      <c r="C585" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="C585" t="n">
+        <v>4</v>
       </c>
       <c r="D585" t="inlineStr">
         <is>
           <t>Baltimore Orioles</t>
         </is>
       </c>
-      <c r="E585" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E585" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="586">
@@ -13907,20 +13903,16 @@
           <t>San Francisco Giants</t>
         </is>
       </c>
-      <c r="C586" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="C586" t="n">
+        <v>1</v>
       </c>
       <c r="D586" t="inlineStr">
         <is>
           <t>Pittsburgh Pirates</t>
         </is>
       </c>
-      <c r="E586" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E586" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="587">
@@ -13934,20 +13926,16 @@
           <t>Philadelphia Phillies</t>
         </is>
       </c>
-      <c r="C587" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C587" t="n">
+        <v>0</v>
       </c>
       <c r="D587" t="inlineStr">
         <is>
           <t>Toronto Blue Jays</t>
         </is>
       </c>
-      <c r="E587" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E587" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="588">
@@ -13961,20 +13949,16 @@
           <t>Los Angeles Angels</t>
         </is>
       </c>
-      <c r="C588" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C588" t="n">
+        <v>0</v>
       </c>
       <c r="D588" t="inlineStr">
         <is>
           <t>Boston Red Sox</t>
         </is>
       </c>
-      <c r="E588" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E588" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="589">
@@ -13988,20 +13972,16 @@
           <t>Chicago Cubs</t>
         </is>
       </c>
-      <c r="C589" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C589" t="n">
+        <v>0</v>
       </c>
       <c r="D589" t="inlineStr">
         <is>
           <t>Detroit Tigers</t>
         </is>
       </c>
-      <c r="E589" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E589" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="590">
@@ -14015,20 +13995,16 @@
           <t>New York Mets</t>
         </is>
       </c>
-      <c r="C590" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C590" t="n">
+        <v>0</v>
       </c>
       <c r="D590" t="inlineStr">
         <is>
           <t>Tampa Bay Rays</t>
         </is>
       </c>
-      <c r="E590" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E590" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="591">
@@ -14042,20 +14018,16 @@
           <t>Kansas City Royals</t>
         </is>
       </c>
-      <c r="C591" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="C591" t="n">
+        <v>1</v>
       </c>
       <c r="D591" t="inlineStr">
         <is>
           <t>Chicago White Sox</t>
         </is>
       </c>
-      <c r="E591" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E591" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="592">
@@ -14069,20 +14041,16 @@
           <t>Texas Rangers</t>
         </is>
       </c>
-      <c r="C592" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C592" t="n">
+        <v>0</v>
       </c>
       <c r="D592" t="inlineStr">
         <is>
           <t>Houston Astros</t>
         </is>
       </c>
-      <c r="E592" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E592" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="593">
@@ -14096,20 +14064,16 @@
           <t>Atlanta Braves</t>
         </is>
       </c>
-      <c r="C593" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C593" t="n">
+        <v>0</v>
       </c>
       <c r="D593" t="inlineStr">
         <is>
           <t>Milwaukee Brewers</t>
         </is>
       </c>
-      <c r="E593" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E593" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="594">
@@ -14123,20 +14087,16 @@
           <t>Oakland Athletics</t>
         </is>
       </c>
-      <c r="C594" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C594" t="n">
+        <v>0</v>
       </c>
       <c r="D594" t="inlineStr">
         <is>
           <t>Minnesota Twins</t>
         </is>
       </c>
-      <c r="E594" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E594" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="595">
@@ -14150,20 +14110,16 @@
           <t>Cincinnati Reds</t>
         </is>
       </c>
-      <c r="C595" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C595" t="n">
+        <v>0</v>
       </c>
       <c r="D595" t="inlineStr">
         <is>
           <t>Colorado Rockies</t>
         </is>
       </c>
-      <c r="E595" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E595" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="596">
@@ -14177,20 +14133,16 @@
           <t>Washington Nationals</t>
         </is>
       </c>
-      <c r="C596" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C596" t="n">
+        <v>0</v>
       </c>
       <c r="D596" t="inlineStr">
         <is>
           <t>Arizona Diamondbacks</t>
         </is>
       </c>
-      <c r="E596" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E596" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="597">
@@ -14204,20 +14156,16 @@
           <t>Miami Marlins</t>
         </is>
       </c>
-      <c r="C597" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C597" t="n">
+        <v>0</v>
       </c>
       <c r="D597" t="inlineStr">
         <is>
           <t>Los Angeles Dodgers</t>
         </is>
       </c>
-      <c r="E597" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E597" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="598">
@@ -14231,20 +14179,16 @@
           <t>Cleveland Indians</t>
         </is>
       </c>
-      <c r="C598" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C598" t="n">
+        <v>0</v>
       </c>
       <c r="D598" t="inlineStr">
         <is>
           <t>Seattle Mariners</t>
         </is>
       </c>
-      <c r="E598" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E598" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="599">
@@ -14258,17 +14202,625 @@
           <t>St. Louis Cardinals</t>
         </is>
       </c>
-      <c r="C599" t="inlineStr">
+      <c r="C599" t="n">
+        <v>2</v>
+      </c>
+      <c r="D599" t="inlineStr">
+        <is>
+          <t>San Diego Padres</t>
+        </is>
+      </c>
+      <c r="E599" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>Monday, May 17, 2021</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>San Francisco Giants</t>
+        </is>
+      </c>
+      <c r="C600" t="n">
+        <v>1</v>
+      </c>
+      <c r="D600" t="inlineStr">
+        <is>
+          <t>Cincinnati Reds</t>
+        </is>
+      </c>
+      <c r="E600" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>Monday, May 17, 2021</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>New York Mets</t>
+        </is>
+      </c>
+      <c r="C601" t="n">
+        <v>0</v>
+      </c>
+      <c r="D601" t="inlineStr">
+        <is>
+          <t>Atlanta Braves</t>
+        </is>
+      </c>
+      <c r="E601" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>Monday, May 17, 2021</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Washington Nationals</t>
+        </is>
+      </c>
+      <c r="C602" t="n">
+        <v>0</v>
+      </c>
+      <c r="D602" t="inlineStr">
+        <is>
+          <t>Chicago Cubs</t>
+        </is>
+      </c>
+      <c r="E602" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>Monday, May 17, 2021</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Chicago White Sox</t>
+        </is>
+      </c>
+      <c r="C603" t="n">
+        <v>3</v>
+      </c>
+      <c r="D603" t="inlineStr">
+        <is>
+          <t>Minnesota Twins</t>
+        </is>
+      </c>
+      <c r="E603" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>Monday, May 17, 2021</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>New York Yankees</t>
+        </is>
+      </c>
+      <c r="C604" t="n">
+        <v>1</v>
+      </c>
+      <c r="D604" t="inlineStr">
+        <is>
+          <t>Texas Rangers</t>
+        </is>
+      </c>
+      <c r="E604" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>Monday, May 17, 2021</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Cleveland Indians</t>
+        </is>
+      </c>
+      <c r="C605" t="n">
+        <v>1</v>
+      </c>
+      <c r="D605" t="inlineStr">
+        <is>
+          <t>Los Angeles Angels</t>
+        </is>
+      </c>
+      <c r="E605" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>Monday, May 17, 2021</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Arizona Diamondbacks</t>
+        </is>
+      </c>
+      <c r="C606" t="n">
+        <v>0</v>
+      </c>
+      <c r="D606" t="inlineStr">
+        <is>
+          <t>Los Angeles Dodgers</t>
+        </is>
+      </c>
+      <c r="E606" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>Monday, May 17, 2021</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Colorado Rockies</t>
+        </is>
+      </c>
+      <c r="C607" t="n">
+        <v>0</v>
+      </c>
+      <c r="D607" t="inlineStr">
+        <is>
+          <t>San Diego Padres</t>
+        </is>
+      </c>
+      <c r="E607" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>Monday, May 17, 2021</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Detroit Tigers</t>
+        </is>
+      </c>
+      <c r="C608" t="n">
+        <v>0</v>
+      </c>
+      <c r="D608" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="E608" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>San Francisco Giants</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D609" t="inlineStr">
+        <is>
+          <t>Cincinnati Reds</t>
+        </is>
+      </c>
+      <c r="E609" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Tampa Bay Rays</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D610" t="inlineStr">
+        <is>
+          <t>Baltimore Orioles</t>
+        </is>
+      </c>
+      <c r="E610" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Miami Marlins</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D611" t="inlineStr">
+        <is>
+          <t>Philadelphia Phillies</t>
+        </is>
+      </c>
+      <c r="E611" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>New York Mets</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D612" t="inlineStr">
+        <is>
+          <t>Atlanta Braves</t>
+        </is>
+      </c>
+      <c r="E612" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Boston Red Sox</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D613" t="inlineStr">
+        <is>
+          <t>Toronto Blue Jays</t>
+        </is>
+      </c>
+      <c r="E613" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Washington Nationals</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D614" t="inlineStr">
+        <is>
+          <t>Chicago Cubs</t>
+        </is>
+      </c>
+      <c r="E614" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Chicago White Sox</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D615" t="inlineStr">
+        <is>
+          <t>Minnesota Twins</t>
+        </is>
+      </c>
+      <c r="E615" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Pittsburgh Pirates</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D616" t="inlineStr">
+        <is>
+          <t>St. Louis Cardinals</t>
+        </is>
+      </c>
+      <c r="E616" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="D599" t="inlineStr">
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>New York Yankees</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D617" t="inlineStr">
+        <is>
+          <t>Texas Rangers</t>
+        </is>
+      </c>
+      <c r="E617" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Milwaukee Brewers</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D618" t="inlineStr">
+        <is>
+          <t>Kansas City Royals</t>
+        </is>
+      </c>
+      <c r="E618" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Cleveland Indians</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D619" t="inlineStr">
+        <is>
+          <t>Los Angeles Angels</t>
+        </is>
+      </c>
+      <c r="E619" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Houston Astros</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D620" t="inlineStr">
+        <is>
+          <t>Oakland Athletics</t>
+        </is>
+      </c>
+      <c r="E620" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Arizona Diamondbacks</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D621" t="inlineStr">
+        <is>
+          <t>Los Angeles Dodgers</t>
+        </is>
+      </c>
+      <c r="E621" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Colorado Rockies</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D622" t="inlineStr">
         <is>
           <t>San Diego Padres</t>
         </is>
       </c>
-      <c r="E599" t="inlineStr">
+      <c r="E622" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>Tuesday, May 18, 2021</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Detroit Tigers</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D623" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="E623" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>